<commit_message>
add(not working yet) class to hold lin regressions
</commit_message>
<xml_diff>
--- a/Othello/linear-regression-results.xlsx
+++ b/Othello/linear-regression-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hailiemitchell/Documents/Dickinson/2022 Fall/COMP 364/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hailiemitchell/Documents/Dickinson/2022 Fall/COMP 364/Othello-Optimization/Othello/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942E89D2-E82A-C442-92F2-B7CCC91F888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A56630-0FED-D248-AA72-A84F7A290AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D427E389-F4AB-4249-B452-BA09B9D5A083}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{D427E389-F4AB-4249-B452-BA09B9D5A083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,49 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>num obsv.</t>
-  </si>
-  <si>
-    <t>Int</t>
-  </si>
-  <si>
-    <t>v' coeff</t>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>^2</t>
-    </r>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -418,830 +387,830 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF05FC43-EF4C-1443-A44F-4542965792B3}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>2002</v>
+      </c>
+      <c r="C1">
+        <v>8</v>
+      </c>
+      <c r="D1">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>9.0052599999999998</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-1.317E-3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6.1770000000000003E-7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="C3">
-        <v>9.0052599999999998</v>
+        <v>7.5056500000000002</v>
       </c>
       <c r="D3">
-        <v>-1.317E-3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>6.1770000000000003E-7</v>
+        <v>0.49886999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.25130000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>2002</v>
+        <v>1873</v>
       </c>
       <c r="C4">
-        <v>7.5056500000000002</v>
+        <v>10.24264</v>
       </c>
       <c r="D4">
-        <v>0.49886999999999998</v>
+        <v>0.27242</v>
       </c>
       <c r="E4">
-        <v>0.25130000000000002</v>
+        <v>3.1570000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1873</v>
+        <v>1778</v>
       </c>
       <c r="C5">
-        <v>10.24264</v>
+        <v>12.3642</v>
       </c>
       <c r="D5">
-        <v>0.27242</v>
+        <v>2.0230000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>3.1570000000000001E-2</v>
+        <v>2.2690000000000001E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1778</v>
+        <v>1935</v>
       </c>
       <c r="C6">
-        <v>12.3642</v>
+        <v>13.25188</v>
       </c>
       <c r="D6">
-        <v>2.0230000000000001E-2</v>
+        <v>-4.0399999999999998E-2</v>
       </c>
       <c r="E6">
-        <v>2.2690000000000001E-4</v>
+        <v>1.2160000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>1935</v>
+        <v>1788</v>
       </c>
       <c r="C7">
-        <v>13.25188</v>
+        <v>13.5883</v>
       </c>
       <c r="D7">
-        <v>-4.0399999999999998E-2</v>
+        <v>8.516E-2</v>
       </c>
       <c r="E7">
-        <v>1.2160000000000001E-3</v>
+        <v>8.6110000000000006E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>1788</v>
+        <v>1868</v>
       </c>
       <c r="C8">
-        <v>13.5883</v>
+        <v>15.36411</v>
       </c>
       <c r="D8">
-        <v>8.516E-2</v>
+        <v>-4.9669999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>8.6110000000000006E-3</v>
+        <v>2.5249999999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>1868</v>
+        <v>1729</v>
       </c>
       <c r="C9">
-        <v>15.36411</v>
+        <v>14.272869999999999</v>
       </c>
       <c r="D9">
-        <v>-4.9669999999999999E-2</v>
+        <v>0.17466999999999999</v>
       </c>
       <c r="E9">
-        <v>2.5249999999999999E-3</v>
+        <v>6.9849999999999995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>1729</v>
+        <v>1868</v>
       </c>
       <c r="C10">
-        <v>14.272869999999999</v>
+        <v>17.17737</v>
       </c>
       <c r="D10">
-        <v>0.17466999999999999</v>
+        <v>-5.339E-2</v>
       </c>
       <c r="E10">
-        <v>6.9849999999999995E-2</v>
+        <v>3.2620000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>1868</v>
+        <v>1759</v>
       </c>
       <c r="C11">
-        <v>17.17737</v>
+        <v>15.24675</v>
       </c>
       <c r="D11">
-        <v>-5.339E-2</v>
+        <v>0.21462000000000001</v>
       </c>
       <c r="E11">
-        <v>3.2620000000000001E-3</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>1759</v>
+        <v>1848</v>
       </c>
       <c r="C12">
-        <v>15.24675</v>
+        <v>18.564979999999998</v>
       </c>
       <c r="D12">
-        <v>0.21462000000000001</v>
+        <v>-2.5930000000000002E-2</v>
       </c>
       <c r="E12">
-        <v>0.1104</v>
+        <v>8.742E-4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
-        <v>1848</v>
+        <v>1762</v>
       </c>
       <c r="C13">
-        <v>18.564979999999998</v>
+        <v>16.173349999999999</v>
       </c>
       <c r="D13">
-        <v>-2.5930000000000002E-2</v>
+        <v>0.25377</v>
       </c>
       <c r="E13">
-        <v>8.742E-4</v>
+        <v>0.13689999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>1762</v>
+        <v>1863</v>
       </c>
       <c r="C14">
-        <v>16.173349999999999</v>
+        <v>18.930019999999999</v>
       </c>
       <c r="D14">
-        <v>0.25377</v>
+        <v>8.8910000000000003E-2</v>
       </c>
       <c r="E14">
-        <v>0.13689999999999999</v>
+        <v>1.295E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>1863</v>
+        <v>1791</v>
       </c>
       <c r="C15">
-        <v>18.930019999999999</v>
+        <v>17.478349999999999</v>
       </c>
       <c r="D15">
-        <v>8.8910000000000003E-2</v>
+        <v>0.25657999999999997</v>
       </c>
       <c r="E15">
-        <v>1.295E-2</v>
+        <v>0.15989999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>1791</v>
+        <v>1867</v>
       </c>
       <c r="C16">
-        <v>17.478349999999999</v>
+        <v>19.28576</v>
       </c>
       <c r="D16">
-        <v>0.25657999999999997</v>
+        <v>0.1794</v>
       </c>
       <c r="E16">
-        <v>0.15989999999999999</v>
+        <v>5.8040000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>1867</v>
+        <v>1774</v>
       </c>
       <c r="C17">
-        <v>19.28576</v>
+        <v>18.092140000000001</v>
       </c>
       <c r="D17">
-        <v>0.1794</v>
+        <v>0.30556</v>
       </c>
       <c r="E17">
-        <v>5.8040000000000001E-2</v>
+        <v>0.21079999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>1774</v>
+        <v>1850</v>
       </c>
       <c r="C18">
-        <v>18.092140000000001</v>
+        <v>19.47139</v>
       </c>
       <c r="D18">
-        <v>0.30556</v>
+        <v>0.26351000000000002</v>
       </c>
       <c r="E18">
-        <v>0.21079999999999999</v>
+        <v>0.1258</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>1850</v>
+        <v>1778</v>
       </c>
       <c r="C19">
-        <v>19.47139</v>
+        <v>19.121410000000001</v>
       </c>
       <c r="D19">
-        <v>0.26351000000000002</v>
+        <v>0.31852999999999998</v>
       </c>
       <c r="E19">
-        <v>0.1258</v>
+        <v>0.22520000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>1778</v>
+        <v>1869</v>
       </c>
       <c r="C20">
-        <v>19.121410000000001</v>
+        <v>20.681380000000001</v>
       </c>
       <c r="D20">
-        <v>0.31852999999999998</v>
+        <v>0.26862999999999998</v>
       </c>
       <c r="E20">
-        <v>0.22520000000000001</v>
+        <v>0.15759999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21">
-        <v>1869</v>
+        <v>1791</v>
       </c>
       <c r="C21">
-        <v>20.681380000000001</v>
+        <v>19.571100000000001</v>
       </c>
       <c r="D21">
-        <v>0.26862999999999998</v>
+        <v>0.35930000000000001</v>
       </c>
       <c r="E21">
-        <v>0.15759999999999999</v>
+        <v>0.26910000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22">
-        <v>1791</v>
+        <v>1893</v>
       </c>
       <c r="C22">
-        <v>19.571100000000001</v>
+        <v>21.538599999999999</v>
       </c>
       <c r="D22">
-        <v>0.35930000000000001</v>
+        <v>0.29449999999999998</v>
       </c>
       <c r="E22">
-        <v>0.26910000000000001</v>
+        <v>0.1918</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
-        <v>1893</v>
+        <v>1800</v>
       </c>
       <c r="C23">
-        <v>21.538599999999999</v>
+        <v>20.640899999999998</v>
       </c>
       <c r="D23">
-        <v>0.29449999999999998</v>
+        <v>0.3654</v>
       </c>
       <c r="E23">
-        <v>0.1918</v>
+        <v>0.28060000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24">
-        <v>1800</v>
+        <v>1910</v>
       </c>
       <c r="C24">
-        <v>20.640899999999998</v>
+        <v>21.867260000000002</v>
       </c>
       <c r="D24">
-        <v>0.3654</v>
+        <v>0.34181</v>
       </c>
       <c r="E24">
-        <v>0.28060000000000002</v>
+        <v>0.2641</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25">
-        <v>1910</v>
+        <v>1806</v>
       </c>
       <c r="C25">
-        <v>21.867260000000002</v>
+        <v>21.163959999999999</v>
       </c>
       <c r="D25">
-        <v>0.34181</v>
+        <v>0.39710000000000001</v>
       </c>
       <c r="E25">
-        <v>0.2641</v>
+        <v>0.30769999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>1806</v>
+        <v>1891</v>
       </c>
       <c r="C26">
-        <v>21.163959999999999</v>
+        <v>22.540469999999999</v>
       </c>
       <c r="D26">
-        <v>0.39710000000000001</v>
+        <v>0.36558000000000002</v>
       </c>
       <c r="E26">
-        <v>0.30769999999999997</v>
+        <v>0.29649999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27">
-        <v>1891</v>
+        <v>1810</v>
       </c>
       <c r="C27">
-        <v>22.540469999999999</v>
+        <v>21.679220000000001</v>
       </c>
       <c r="D27">
-        <v>0.36558000000000002</v>
+        <v>0.42343999999999998</v>
       </c>
       <c r="E27">
-        <v>0.29649999999999999</v>
+        <v>0.31900000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28">
-        <v>1810</v>
+        <v>1895</v>
       </c>
       <c r="C28">
-        <v>21.679220000000001</v>
+        <v>22.909770000000002</v>
       </c>
       <c r="D28">
-        <v>0.42343999999999998</v>
+        <v>0.39678999999999998</v>
       </c>
       <c r="E28">
-        <v>0.31900000000000001</v>
+        <v>0.34050000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29">
-        <v>1895</v>
+        <v>1815</v>
       </c>
       <c r="C29">
-        <v>22.909770000000002</v>
+        <v>22.67501</v>
       </c>
       <c r="D29">
-        <v>0.39678999999999998</v>
+        <v>0.42210999999999999</v>
       </c>
       <c r="E29">
-        <v>0.34050000000000002</v>
+        <v>0.3342</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>1815</v>
+        <v>1908</v>
       </c>
       <c r="C30">
-        <v>22.67501</v>
+        <v>23.421659999999999</v>
       </c>
       <c r="D30">
-        <v>0.42210999999999999</v>
+        <v>0.42007</v>
       </c>
       <c r="E30">
-        <v>0.3342</v>
+        <v>0.36170000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>1908</v>
+        <v>1809</v>
       </c>
       <c r="C31">
-        <v>23.421659999999999</v>
+        <v>23.189319999999999</v>
       </c>
       <c r="D31">
-        <v>0.42007</v>
+        <v>0.44261</v>
       </c>
       <c r="E31">
-        <v>0.36170000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32">
-        <v>1809</v>
+        <v>1912</v>
       </c>
       <c r="C32">
-        <v>23.189319999999999</v>
+        <v>24.0962</v>
       </c>
       <c r="D32">
-        <v>0.44261</v>
+        <v>0.43240000000000001</v>
       </c>
       <c r="E32">
-        <v>0.36199999999999999</v>
+        <v>0.38519999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33">
-        <v>1912</v>
+        <v>1811</v>
       </c>
       <c r="C33">
-        <v>24.0962</v>
+        <v>23.623390000000001</v>
       </c>
       <c r="D33">
-        <v>0.43240000000000001</v>
+        <v>0.46028999999999998</v>
       </c>
       <c r="E33">
-        <v>0.38519999999999999</v>
+        <v>0.372</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34">
-        <v>1811</v>
+        <v>1913</v>
       </c>
       <c r="C34">
-        <v>23.623390000000001</v>
+        <v>24.591000000000001</v>
       </c>
       <c r="D34">
-        <v>0.46028999999999998</v>
+        <v>0.44650000000000001</v>
       </c>
       <c r="E34">
-        <v>0.372</v>
+        <v>0.3926</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35">
-        <v>1913</v>
+        <v>1810</v>
       </c>
       <c r="C35">
-        <v>24.591000000000001</v>
+        <v>23.235060000000001</v>
       </c>
       <c r="D35">
-        <v>0.44650000000000001</v>
+        <v>0.50771999999999995</v>
       </c>
       <c r="E35">
-        <v>0.3926</v>
+        <v>0.42149999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36">
-        <v>1810</v>
+        <v>1912</v>
       </c>
       <c r="C36">
-        <v>23.235060000000001</v>
+        <v>25.57349</v>
       </c>
       <c r="D36">
-        <v>0.50771999999999995</v>
+        <v>0.44157000000000002</v>
       </c>
       <c r="E36">
-        <v>0.42149999999999999</v>
+        <v>0.37230000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37">
-        <v>1912</v>
+        <v>1806</v>
       </c>
       <c r="C37">
-        <v>25.57349</v>
+        <v>24.51511</v>
       </c>
       <c r="D37">
-        <v>0.44157000000000002</v>
+        <v>0.49067</v>
       </c>
       <c r="E37">
-        <v>0.37230000000000002</v>
+        <v>0.38740000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>1806</v>
+        <v>1905</v>
       </c>
       <c r="C38">
-        <v>24.51511</v>
+        <v>25.588509999999999</v>
       </c>
       <c r="D38">
-        <v>0.49067</v>
+        <v>0.4703</v>
       </c>
       <c r="E38">
-        <v>0.38740000000000002</v>
+        <v>0.37619999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39">
-        <v>1905</v>
+        <v>1810</v>
       </c>
       <c r="C39">
-        <v>25.588509999999999</v>
+        <v>24.173719999999999</v>
       </c>
       <c r="D39">
-        <v>0.4703</v>
+        <v>0.5292</v>
       </c>
       <c r="E39">
-        <v>0.37619999999999998</v>
+        <v>0.4158</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40">
-        <v>1810</v>
+        <v>1909</v>
       </c>
       <c r="C40">
-        <v>24.173719999999999</v>
+        <v>26.938580000000002</v>
       </c>
       <c r="D40">
-        <v>0.5292</v>
+        <v>0.45162999999999998</v>
       </c>
       <c r="E40">
-        <v>0.4158</v>
+        <v>0.36059999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41">
-        <v>1909</v>
+        <v>1817</v>
       </c>
       <c r="C41">
-        <v>26.938580000000002</v>
+        <v>24.301110000000001</v>
       </c>
       <c r="D41">
-        <v>0.45162999999999998</v>
+        <v>0.54793999999999998</v>
       </c>
       <c r="E41">
-        <v>0.36059999999999998</v>
+        <v>0.4456</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42">
-        <v>1817</v>
+        <v>1904</v>
       </c>
       <c r="C42">
-        <v>24.301110000000001</v>
+        <v>26.031099999999999</v>
       </c>
       <c r="D42">
-        <v>0.54793999999999998</v>
+        <v>0.50019999999999998</v>
       </c>
       <c r="E42">
-        <v>0.4456</v>
+        <v>0.38490000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43">
-        <v>1904</v>
+        <v>1812</v>
       </c>
       <c r="C43">
-        <v>26.031099999999999</v>
+        <v>23.960629999999998</v>
       </c>
       <c r="D43">
-        <v>0.50019999999999998</v>
+        <v>0.57460999999999995</v>
       </c>
       <c r="E43">
-        <v>0.38490000000000002</v>
+        <v>0.44850000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44">
-        <v>1812</v>
+        <v>1896</v>
       </c>
       <c r="C44">
-        <v>23.960629999999998</v>
+        <v>26.08399</v>
       </c>
       <c r="D44">
-        <v>0.57460999999999995</v>
+        <v>0.52059</v>
       </c>
       <c r="E44">
-        <v>0.44850000000000001</v>
+        <v>0.39319999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45">
-        <v>1896</v>
+        <v>1804</v>
       </c>
       <c r="C45">
-        <v>26.08399</v>
+        <v>24.5687</v>
       </c>
       <c r="D45">
-        <v>0.52059</v>
+        <v>0.57452999999999999</v>
       </c>
       <c r="E45">
-        <v>0.39319999999999999</v>
+        <v>0.44140000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46">
-        <v>1804</v>
+        <v>1902</v>
       </c>
       <c r="C46">
-        <v>24.5687</v>
+        <v>27.72316</v>
       </c>
       <c r="D46">
-        <v>0.57452999999999999</v>
+        <v>0.48594999999999999</v>
       </c>
       <c r="E46">
-        <v>0.44140000000000001</v>
+        <v>0.34610000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47">
-        <v>1902</v>
+        <v>1803</v>
       </c>
       <c r="C47">
-        <v>27.72316</v>
+        <v>26.969860000000001</v>
       </c>
       <c r="D47">
-        <v>0.48594999999999999</v>
+        <v>0.51815</v>
       </c>
       <c r="E47">
-        <v>0.34610000000000002</v>
+        <v>0.37459999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48">
-        <v>1803</v>
+        <v>1897</v>
       </c>
       <c r="C48">
-        <v>26.969860000000001</v>
+        <v>28.536210000000001</v>
       </c>
       <c r="D48">
-        <v>0.51815</v>
+        <v>0.47728999999999999</v>
       </c>
       <c r="E48">
-        <v>0.37459999999999999</v>
+        <v>0.32469999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>1897</v>
@@ -1258,86 +1227,69 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50">
-        <v>1897</v>
+        <v>1882</v>
       </c>
       <c r="C50">
-        <v>28.536210000000001</v>
+        <v>30.370270000000001</v>
       </c>
       <c r="D50">
-        <v>0.47728999999999999</v>
+        <v>0.43308000000000002</v>
       </c>
       <c r="E50">
-        <v>0.32469999999999999</v>
+        <v>0.27339999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51">
-        <v>1882</v>
+        <v>1766</v>
       </c>
       <c r="C51">
-        <v>30.370270000000001</v>
+        <v>32.870890000000003</v>
       </c>
       <c r="D51">
-        <v>0.43308000000000002</v>
+        <v>0.37124000000000001</v>
       </c>
       <c r="E51">
-        <v>0.27339999999999998</v>
+        <v>0.19159999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52">
-        <v>1766</v>
+        <v>1792</v>
       </c>
       <c r="C52">
-        <v>32.870890000000003</v>
+        <v>37.797130000000003</v>
       </c>
       <c r="D52">
-        <v>0.37124000000000001</v>
+        <v>0.23735999999999999</v>
       </c>
       <c r="E52">
-        <v>0.19159999999999999</v>
+        <v>7.4510000000000007E-2</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53">
-        <v>1792</v>
+        <v>1377</v>
       </c>
       <c r="C53">
-        <v>37.797130000000003</v>
+        <v>46.253990000000002</v>
       </c>
       <c r="D53">
-        <v>0.23735999999999999</v>
+        <v>3.6700000000000003E-2</v>
       </c>
       <c r="E53">
-        <v>7.4510000000000007E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>56</v>
-      </c>
-      <c r="B54">
-        <v>1377</v>
-      </c>
-      <c r="C54">
-        <v>46.253990000000002</v>
-      </c>
-      <c r="D54">
-        <v>3.6700000000000003E-2</v>
-      </c>
-      <c r="E54">
         <v>1.6100000000000001E-3</v>
       </c>
     </row>

</xml_diff>